<commit_message>
added new test cases
</commit_message>
<xml_diff>
--- a/CTDC_Automation/InputFiles/TC07_Canine_Filter_Breed-Akita.xlsx
+++ b/CTDC_Automation/InputFiles/TC07_Canine_Filter_Breed-Akita.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Script\DataCommons_Automation\CTDC_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233AD39E-63E0-4747-97B1-9107351BE77F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1841AC-68BC-4FBB-A384-86C6BAA041FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Commiting to a stable branch
</commit_message>
<xml_diff>
--- a/CTDC_Automation/InputFiles/TC07_Canine_Filter_Breed-Akita.xlsx
+++ b/CTDC_Automation/InputFiles/TC07_Canine_Filter_Breed-Akita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\DataCommons_Automation\CTDC_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1841AC-68BC-4FBB-A384-86C6BAA041FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D21F11B-D6A5-4194-9919-9FED4C0B76E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Url</t>
   </si>
@@ -52,6 +52,10 @@
   </si>
   <si>
     <t>TC07_Canine_Filter_Breed-Akita_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['Akita'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`
+</t>
   </si>
 </sst>
 </file>
@@ -460,11 +464,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>

</xml_diff>